<commit_message>
config stepDefinitions y parametrización datos de entrada
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\MercadoLibre-Screenplay\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD62C6D-C1C0-441E-BBF1-D833C8477020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5CCFDD-1056-4AC1-BC4B-BA9A490B47E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>url</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>paangudi3@gmail.com</t>
-  </si>
-  <si>
-    <t>Clave</t>
-  </si>
-  <si>
-    <t>Scant9756</t>
   </si>
 </sst>
 </file>
@@ -393,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E6:E7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,10 +398,10 @@
     <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,11 +411,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -430,9 +421,6 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task buscar producto completada
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\MercadoLibre-Screenplay\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5CCFDD-1056-4AC1-BC4B-BA9A490B47E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545D4F73-6009-4886-96AB-68508B1BEEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>url</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>paangudi3@gmail.com</t>
+  </si>
+  <si>
+    <t>Cámara Fujifilm Instax Mini 12 Color Rosa</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -106,6 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -387,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,12 +427,25 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{763E89BB-D89E-4A0B-9CD5-DCE59E274BAD}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{9D4CC1B4-7B66-4298-A355-882F7B65A560}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{7DABD062-12A5-437E-B0FE-0995F1182300}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{61109232-CB36-45AF-84A2-80680D8843CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
validación del producto en resultados busqueda
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\MercadoLibre-Screenplay\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545D4F73-6009-4886-96AB-68508B1BEEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152D558-02D3-4C08-87DB-7C4502071132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>url</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>paangudi3@gmail.com</t>
-  </si>
-  <si>
-    <t>Cámara Fujifilm Instax Mini 12 Color Rosa</t>
   </si>
 </sst>
 </file>
@@ -98,7 +95,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -109,7 +106,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -391,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,25 +423,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{763E89BB-D89E-4A0B-9CD5-DCE59E274BAD}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{9D4CC1B4-7B66-4298-A355-882F7B65A560}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{7DABD062-12A5-437E-B0FE-0995F1182300}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{61109232-CB36-45AF-84A2-80680D8843CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
configuracion entorno inicio de sesion
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\MercadoLibre-Screenplay\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152D558-02D3-4C08-87DB-7C4502071132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B320DFB-3A1C-4296-B99B-3306F9BC4878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>url</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>paangudi3@gmail.com</t>
+  </si>
+  <si>
+    <t>clave</t>
+  </si>
+  <si>
+    <t>Scant9756</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,10 +404,10 @@
     <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,8 +417,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -421,6 +430,9 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
config mapeo de datos
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\MercadoLibre-Screenplay\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC2A16-7BC5-4DBC-AE3F-6D781A0FB7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814EA8AB-C671-4D58-BAA6-08ABD5410167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>url</t>
   </si>
@@ -43,15 +43,6 @@
   </si>
   <si>
     <t>Crear cuenta</t>
-  </si>
-  <si>
-    <t>Camara Fujifilm Instax Mini 12 Morada Color Violeta</t>
-  </si>
-  <si>
-    <t>Silla Gamer Premium Elite Cute Stream</t>
-  </si>
-  <si>
-    <t>Ingresar</t>
   </si>
 </sst>
 </file>
@@ -104,7 +95,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -114,10 +105,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -400,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,35 +422,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{763E89BB-D89E-4A0B-9CD5-DCE59E274BAD}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{F257D26C-B972-4D37-A68A-0812D926A202}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{388D4DB3-651F-4D01-9C71-9A3C8370A3E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>